<commit_message>
Commit all changes till Contact Us using Nunit Framework
</commit_message>
<xml_diff>
--- a/SFS_SmokeTest/TestCases_Docs/ATX_P0testcases.xlsx
+++ b/SFS_SmokeTest/TestCases_Docs/ATX_P0testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Framework\GitHub\AutomationSuiteCSharp_SFS\SFS_SmokeTest\TestCases_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE54F0B-D04D-42C3-93AF-7A706ABD8E8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F72994C-CEC2-434F-A005-BBD20FF4BF7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B389FAE1-FDED-4610-8300-114D2B489EFF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="163">
   <si>
     <t>Sr no</t>
   </si>
@@ -174,15 +174,6 @@
     <t xml:space="preserve">User should be successfully redirected to https://wdc-qa-support.atxinc.com/communities/index. </t>
   </si>
   <si>
-    <t>Verify user is successfully redirected to My Account  page and validate the URL https://wdc-qa-support.atxinc.com/myinformation/myaccount?redirectToSSPMYA=true</t>
-  </si>
-  <si>
-    <t>User should be successfully redirected to https://wdc-qa-support.atxinc.com/myinformation/myaccount?redirectToSSPMYA=true.</t>
-  </si>
-  <si>
-    <t>Verify user is successfully redirected to Chat live with a CCH Expert page and validate the URL https://support-demo.cch.com/sfs/taxwisechat</t>
-  </si>
-  <si>
     <t>1. Goto ATX Home Page.
 2. Click on Chat Link</t>
   </si>
@@ -194,16 +185,10 @@
 2. Click on Open Link</t>
   </si>
   <si>
-    <t>Verify user is successfully redirected to Open a support case page and validate the https://support-demo.cch.com/sfs/ContactUs.aspx?id=TlLoJ8WbVPxqCkeeYjyd9dFrXa6IR9NgHxSNBBIcoUHJ6YLu%2f9E7LcjcqgoHr8Ay25DMj0t0rhvQb4AxEXEAigXDqLNTb2o%2fczjRsu8884M%3d&amp;account=sFHdgT2kYqImepp8b%2bI6%2fa8S8ZEcIHtTq36D%2fopnxmw%3d&amp;returnUrl=http%3a%2f%2fwdc-qa-support.atxinc.com%2fhome%2fhome%3fcode%3ds&amp;errorUrl=http%3a%2f%2fwdc-qa-support.atxinc.com%2fhome%2fhome%3fcode%3de</t>
-  </si>
-  <si>
     <t>1. Goto ATX Home Page.
 2. Click on Click Link</t>
   </si>
   <si>
-    <t>User should be successfully redirected to  https://support-demo.cch.com/sfs/ContactUs.aspx?id=TlLoJ8WbVPxqCkeeYjyd9dFrXa6IR9NgHxSNBBIcoUHJ6YLu%2f9E7LcjcqgoHr8Ay25DMj0t0rhvQb4AxEXEAigXDqLNTb2o%2fczjRsu8884M%3d&amp;account=sFHdgT2kYqImepp8b%2bI6%2fa8S8ZEcIHtTq36D%2fopnxmw%3d&amp;returnUrl=http%3a%2f%2fwdc-qa-support.atxinc.com%2fhome%2fhome%3fcode%3ds&amp;errorUrl=http%3a%2f%2fwdc-qa-support.atxinc.com%2fhome%2fhome%3fcode%3de</t>
-  </si>
-  <si>
     <t>Verify user is successfully redirected to Click for support hours page and validate the URL https://support-demo.cch.com/kb/solution/000093021</t>
   </si>
   <si>
@@ -568,6 +553,21 @@
   </si>
   <si>
     <t>Verify user is successfully redirected to KB Search Link page and validate the URL https://support-demo.cch.com/sfs.</t>
+  </si>
+  <si>
+    <t>Verify user is successfully redirected to My Account  page and validate the https://qa-ngmyaccount.gsdwkglobal.com/myaccount/#/saml?idp=atx</t>
+  </si>
+  <si>
+    <t>User should be successfully redirected to https://qa-ngmyaccount.gsdwkglobal.com/myaccount/#/saml?idp=atx.</t>
+  </si>
+  <si>
+    <t>Verify user is successfully redirected to Open a support case page and validate the https://support-demo.cch.com/sfs/ContactUs.aspx</t>
+  </si>
+  <si>
+    <t>Verify user is successfully redirected to Chat live with a CCH Expert page and validate the URL https://support-demo.cch.com/sfs/atxchat</t>
+  </si>
+  <si>
+    <t>User should be successfully redirected to  https://support-demo.cch.com/sfs/ContactUs.aspx?</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A9A0EA-E752-4DB4-8070-4BB8A6A50C23}">
   <dimension ref="A1:L163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="65" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:K9"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="84" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,7 +1035,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1056,10 +1056,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>7</v>
@@ -1073,12 +1073,12 @@
     </row>
     <row r="2" spans="1:12" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="7" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -1102,7 +1102,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>30</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="4" spans="1:12" s="7" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B4" s="9">
         <v>2</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="5" spans="1:12" s="7" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B5" s="9">
         <v>3</v>
@@ -1174,12 +1174,12 @@
     </row>
     <row r="6" spans="1:12" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9">
         <v>4</v>
@@ -1188,7 +1188,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>22</v>
@@ -1197,13 +1197,13 @@
         <v>20</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>30</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="8" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B8" s="9">
         <v>5</v>
@@ -1237,7 +1237,7 @@
         <v>36</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>30</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="9" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B9" s="9">
         <v>22</v>
@@ -1258,20 +1258,20 @@
         <v>19</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>30</v>
@@ -1283,12 +1283,12 @@
     </row>
     <row r="10" spans="1:12" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B11" s="9">
         <v>6</v>
@@ -1297,7 +1297,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>22</v>
@@ -1307,10 +1307,10 @@
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>30</v>
@@ -1322,7 +1322,7 @@
     </row>
     <row r="12" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B12" s="9">
         <v>7</v>
@@ -1344,7 +1344,7 @@
         <v>28</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>30</v>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="13" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B13" s="9">
         <v>8</v>
@@ -1378,7 +1378,7 @@
         <v>38</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>30</v>
@@ -1390,12 +1390,12 @@
     </row>
     <row r="14" spans="1:12" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B15" s="9">
         <v>9</v>
@@ -1404,7 +1404,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>39</v>
+        <v>158</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>22</v>
@@ -1414,16 +1414,22 @@
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
+        <v>159</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B16" s="9">
         <v>10</v>
@@ -1444,19 +1450,25 @@
       <c r="H16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
+      <c r="I16" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="1:12" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B18" s="9">
         <v>11</v>
@@ -1465,26 +1477,32 @@
         <v>19</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
+        <v>40</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="L18" s="9"/>
     </row>
-    <row r="19" spans="1:12" s="7" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B19" s="9">
         <v>12</v>
@@ -1493,26 +1511,32 @@
         <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
+        <v>162</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="L19" s="9"/>
     </row>
     <row r="20" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B20" s="9">
         <v>13</v>
@@ -1521,31 +1545,37 @@
         <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="L20" s="9"/>
     </row>
     <row r="21" spans="1:12" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B22" s="9">
         <v>14</v>
@@ -1554,17 +1584,17 @@
         <v>19</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -1573,7 +1603,7 @@
     </row>
     <row r="23" spans="1:12" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B23" s="9">
         <v>15</v>
@@ -1582,17 +1612,17 @@
         <v>19</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -1601,7 +1631,7 @@
     </row>
     <row r="24" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B24" s="9">
         <v>16</v>
@@ -1610,17 +1640,17 @@
         <v>19</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -1629,7 +1659,7 @@
     </row>
     <row r="25" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B25" s="9">
         <v>17</v>
@@ -1638,17 +1668,17 @@
         <v>19</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G25" s="9"/>
       <c r="H25" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
@@ -1657,7 +1687,7 @@
     </row>
     <row r="26" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B26" s="9">
         <v>18</v>
@@ -1666,17 +1696,17 @@
         <v>19</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G26" s="9"/>
       <c r="H26" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
@@ -1685,7 +1715,7 @@
     </row>
     <row r="27" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B27" s="9">
         <v>19</v>
@@ -1694,17 +1724,17 @@
         <v>19</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
@@ -1713,7 +1743,7 @@
     </row>
     <row r="28" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B28" s="9">
         <v>20</v>
@@ -1722,17 +1752,17 @@
         <v>19</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
@@ -1741,7 +1771,7 @@
     </row>
     <row r="29" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B29" s="9">
         <v>21</v>
@@ -1750,17 +1780,17 @@
         <v>19</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
@@ -1769,12 +1799,12 @@
     </row>
     <row r="30" spans="1:12" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B31" s="9">
         <v>23</v>
@@ -1783,17 +1813,17 @@
         <v>19</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
@@ -1802,7 +1832,7 @@
     </row>
     <row r="32" spans="1:12" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B32" s="9">
         <v>24</v>
@@ -1811,17 +1841,17 @@
         <v>19</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
@@ -1830,7 +1860,7 @@
     </row>
     <row r="33" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B33" s="9">
         <v>25</v>
@@ -1839,17 +1869,17 @@
         <v>19</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G33" s="9"/>
       <c r="H33" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
@@ -1858,7 +1888,7 @@
     </row>
     <row r="34" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B34" s="9">
         <v>26</v>
@@ -1867,17 +1897,17 @@
         <v>19</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G34" s="9"/>
       <c r="H34" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
@@ -1886,7 +1916,7 @@
     </row>
     <row r="35" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B35" s="9">
         <v>27</v>
@@ -1895,17 +1925,17 @@
         <v>19</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G35" s="9"/>
       <c r="H35" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
@@ -1914,7 +1944,7 @@
     </row>
     <row r="36" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B36" s="9">
         <v>28</v>
@@ -1923,17 +1953,17 @@
         <v>19</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G36" s="9"/>
       <c r="H36" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
@@ -1942,7 +1972,7 @@
     </row>
     <row r="37" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B37" s="9">
         <v>29</v>
@@ -1951,17 +1981,17 @@
         <v>19</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G37" s="9"/>
       <c r="H37" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
@@ -1970,7 +2000,7 @@
     </row>
     <row r="38" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B38" s="9">
         <v>30</v>
@@ -1979,17 +2009,17 @@
         <v>19</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G38" s="9"/>
       <c r="H38" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
@@ -1998,12 +2028,12 @@
     </row>
     <row r="39" spans="1:12" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B40" s="9">
         <v>31</v>
@@ -2012,17 +2042,17 @@
         <v>19</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G40" s="9"/>
       <c r="H40" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
@@ -2031,7 +2061,7 @@
     </row>
     <row r="41" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B41" s="9">
         <v>32</v>
@@ -2040,17 +2070,17 @@
         <v>19</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G41" s="9"/>
       <c r="H41" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
@@ -2059,7 +2089,7 @@
     </row>
     <row r="42" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B42" s="9">
         <v>33</v>
@@ -2068,17 +2098,17 @@
         <v>19</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G42" s="9"/>
       <c r="H42" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
@@ -2087,7 +2117,7 @@
     </row>
     <row r="43" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B43" s="9">
         <v>34</v>
@@ -2096,17 +2126,17 @@
         <v>19</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G43" s="9"/>
       <c r="H43" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
@@ -2115,7 +2145,7 @@
     </row>
     <row r="44" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B44" s="9">
         <v>35</v>
@@ -2124,17 +2154,17 @@
         <v>19</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G44" s="9"/>
       <c r="H44" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>

</xml_diff>